<commit_message>
- Offset changed x64 (Player, Unit and Localplayer is missing) - Changed way to set offsets. Delegates in a dictionary are used - Multiple processes of SC2 possible. But not sure if needed. For now it takes the first entry. - Different versions seem to be needed. Can't access x64 SCII with x64_86 application.
</commit_message>
<xml_diff>
--- a/docs/Minimap - scalling.xlsx
+++ b/docs/Minimap - scalling.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Botton</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>Lava Flow</t>
+  </si>
+  <si>
+    <t>coda LE</t>
   </si>
 </sst>
 </file>
@@ -384,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:C12"/>
+  <dimension ref="A4:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -395,15 +398,18 @@
     <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>8</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -413,8 +419,11 @@
       <c r="C5">
         <v>32768</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>81920</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -424,8 +433,11 @@
       <c r="C6">
         <v>40960</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>65536</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -435,8 +447,11 @@
       <c r="C7">
         <v>778239</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>622591</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -446,8 +461,11 @@
       <c r="C8">
         <v>835583</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>671743</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -459,8 +477,11 @@
         <f>C8-C5</f>
         <v>802815</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>589823</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -472,8 +493,11 @@
         <f>C7-C6</f>
         <v>737279</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>557055</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -484,7 +508,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>

</xml_diff>